<commit_message>
Backlog refinement meeting notes
</commit_message>
<xml_diff>
--- a/meeting-notes/App features.xlsx
+++ b/meeting-notes/App features.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Feature list" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Data" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Feature list" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="Data" sheetId="2" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="20">
   <si>
     <t xml:space="preserve">Feature</t>
   </si>
@@ -36,9 +36,6 @@
   </si>
   <si>
     <t xml:space="preserve">CRUD Trip Management (dates, flights)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Destination Setup (cities)</t>
   </si>
   <si>
     <t xml:space="preserve">Accommodation Setup</t>
@@ -171,20 +168,24 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -260,3158 +261,3256 @@
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
+  <a:themeElements>
+    <a:clrScheme name="LibreOffice">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="000000"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="ffffff"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="18a303"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="0369a3"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="a33e03"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8e03a3"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="c99c00"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="c9211e"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000ee"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="551a8b"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:B1017"/>
+  <dimension ref="A2:B1016"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A19" activeCellId="0" sqref="A19"/>
+      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" customHeight="false" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="133.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="133.85"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="3" t="s">
+      <c r="B8" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="3" t="s">
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="3" t="s">
+      <c r="B9" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="3" t="s">
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="4" t="s">
         <v>12</v>
       </c>
+      <c r="B10" s="4" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="A12" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>12</v>
+      <c r="B12" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="A13" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>10</v>
+      <c r="B13" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="A14" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>10</v>
+      <c r="B14" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+      <c r="A15" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>10</v>
+      <c r="B15" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+      <c r="A16" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>10</v>
+      <c r="B16" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+      <c r="A17" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>10</v>
+      <c r="B17" s="3" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>12</v>
-      </c>
+      <c r="B18" s="3"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="2"/>
+      <c r="B19" s="3"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="2"/>
+      <c r="B20" s="3"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="2"/>
+      <c r="B21" s="3"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="2"/>
+      <c r="B22" s="3"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="2"/>
+      <c r="B23" s="3"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="2"/>
+      <c r="B24" s="3"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="2"/>
+      <c r="B25" s="3"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="2"/>
+      <c r="B26" s="3"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="2"/>
+      <c r="B27" s="3"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="2"/>
+      <c r="B28" s="3"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="2"/>
+      <c r="B29" s="3"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="2"/>
+      <c r="B30" s="3"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="2"/>
+      <c r="B31" s="3"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="2"/>
+      <c r="B32" s="3"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="2"/>
+      <c r="B33" s="3"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="2"/>
+      <c r="B34" s="3"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="2"/>
+      <c r="B35" s="3"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="2"/>
+      <c r="B36" s="3"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B37" s="2"/>
+      <c r="B37" s="3"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="2"/>
+      <c r="B38" s="3"/>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="2"/>
+      <c r="B39" s="3"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B40" s="2"/>
+      <c r="B40" s="3"/>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B41" s="2"/>
+      <c r="B41" s="3"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B42" s="2"/>
+      <c r="B42" s="3"/>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B43" s="2"/>
+      <c r="B43" s="3"/>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B44" s="2"/>
+      <c r="B44" s="3"/>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B45" s="2"/>
+      <c r="B45" s="3"/>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B46" s="2"/>
+      <c r="B46" s="3"/>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B47" s="2"/>
+      <c r="B47" s="3"/>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B48" s="2"/>
+      <c r="B48" s="3"/>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B49" s="2"/>
+      <c r="B49" s="3"/>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B50" s="2"/>
+      <c r="B50" s="3"/>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B51" s="2"/>
+      <c r="B51" s="3"/>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B52" s="2"/>
+      <c r="B52" s="3"/>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B53" s="2"/>
+      <c r="B53" s="3"/>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B54" s="2"/>
+      <c r="B54" s="3"/>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B55" s="2"/>
+      <c r="B55" s="3"/>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B56" s="2"/>
+      <c r="B56" s="3"/>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B57" s="2"/>
+      <c r="B57" s="3"/>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B58" s="2"/>
+      <c r="B58" s="3"/>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B59" s="2"/>
+      <c r="B59" s="3"/>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B60" s="2"/>
+      <c r="B60" s="3"/>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B61" s="2"/>
+      <c r="B61" s="3"/>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B62" s="2"/>
+      <c r="B62" s="3"/>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B63" s="2"/>
+      <c r="B63" s="3"/>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B64" s="2"/>
+      <c r="B64" s="3"/>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B65" s="2"/>
+      <c r="B65" s="3"/>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B66" s="2"/>
+      <c r="B66" s="3"/>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B67" s="2"/>
+      <c r="B67" s="3"/>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B68" s="2"/>
+      <c r="B68" s="3"/>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B69" s="2"/>
+      <c r="B69" s="3"/>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B70" s="2"/>
+      <c r="B70" s="3"/>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B71" s="2"/>
+      <c r="B71" s="3"/>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B72" s="2"/>
+      <c r="B72" s="3"/>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B73" s="2"/>
+      <c r="B73" s="3"/>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B74" s="2"/>
+      <c r="B74" s="3"/>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B75" s="2"/>
+      <c r="B75" s="3"/>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B76" s="2"/>
+      <c r="B76" s="3"/>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B77" s="2"/>
+      <c r="B77" s="3"/>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B78" s="2"/>
+      <c r="B78" s="3"/>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B79" s="2"/>
+      <c r="B79" s="3"/>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B80" s="2"/>
+      <c r="B80" s="3"/>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B81" s="2"/>
+      <c r="B81" s="3"/>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B82" s="2"/>
+      <c r="B82" s="3"/>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B83" s="2"/>
+      <c r="B83" s="3"/>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B84" s="2"/>
+      <c r="B84" s="3"/>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B85" s="2"/>
+      <c r="B85" s="3"/>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B86" s="2"/>
+      <c r="B86" s="3"/>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B87" s="2"/>
+      <c r="B87" s="3"/>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B88" s="2"/>
+      <c r="B88" s="3"/>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B89" s="2"/>
+      <c r="B89" s="3"/>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B90" s="2"/>
+      <c r="B90" s="3"/>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B91" s="2"/>
+      <c r="B91" s="3"/>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B92" s="2"/>
+      <c r="B92" s="3"/>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B93" s="2"/>
+      <c r="B93" s="3"/>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B94" s="2"/>
+      <c r="B94" s="3"/>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B95" s="2"/>
+      <c r="B95" s="3"/>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B96" s="2"/>
+      <c r="B96" s="3"/>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B97" s="2"/>
+      <c r="B97" s="3"/>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B98" s="2"/>
+      <c r="B98" s="3"/>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B99" s="2"/>
+      <c r="B99" s="3"/>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B100" s="2"/>
+      <c r="B100" s="3"/>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B101" s="2"/>
+      <c r="B101" s="3"/>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B102" s="2"/>
+      <c r="B102" s="3"/>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B103" s="2"/>
+      <c r="B103" s="3"/>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B104" s="2"/>
+      <c r="B104" s="3"/>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B105" s="2"/>
+      <c r="B105" s="3"/>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B106" s="2"/>
+      <c r="B106" s="3"/>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B107" s="2"/>
+      <c r="B107" s="3"/>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B108" s="2"/>
+      <c r="B108" s="3"/>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B109" s="2"/>
+      <c r="B109" s="3"/>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B110" s="2"/>
+      <c r="B110" s="3"/>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B111" s="2"/>
+      <c r="B111" s="3"/>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B112" s="2"/>
+      <c r="B112" s="3"/>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B113" s="2"/>
+      <c r="B113" s="3"/>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B114" s="2"/>
+      <c r="B114" s="3"/>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B115" s="2"/>
+      <c r="B115" s="3"/>
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B116" s="2"/>
+      <c r="B116" s="3"/>
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B117" s="2"/>
+      <c r="B117" s="3"/>
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B118" s="2"/>
+      <c r="B118" s="3"/>
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B119" s="2"/>
+      <c r="B119" s="3"/>
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B120" s="2"/>
+      <c r="B120" s="3"/>
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B121" s="2"/>
+      <c r="B121" s="3"/>
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B122" s="2"/>
+      <c r="B122" s="3"/>
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B123" s="2"/>
+      <c r="B123" s="3"/>
     </row>
     <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B124" s="2"/>
+      <c r="B124" s="3"/>
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B125" s="2"/>
+      <c r="B125" s="3"/>
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B126" s="2"/>
+      <c r="B126" s="3"/>
     </row>
     <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B127" s="2"/>
+      <c r="B127" s="3"/>
     </row>
     <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B128" s="2"/>
+      <c r="B128" s="3"/>
     </row>
     <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B129" s="2"/>
+      <c r="B129" s="3"/>
     </row>
     <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B130" s="2"/>
+      <c r="B130" s="3"/>
     </row>
     <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B131" s="2"/>
+      <c r="B131" s="3"/>
     </row>
     <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B132" s="2"/>
+      <c r="B132" s="3"/>
     </row>
     <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B133" s="2"/>
+      <c r="B133" s="3"/>
     </row>
     <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B134" s="2"/>
+      <c r="B134" s="3"/>
     </row>
     <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B135" s="2"/>
+      <c r="B135" s="3"/>
     </row>
     <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B136" s="2"/>
+      <c r="B136" s="3"/>
     </row>
     <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B137" s="2"/>
+      <c r="B137" s="3"/>
     </row>
     <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B138" s="2"/>
+      <c r="B138" s="3"/>
     </row>
     <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B139" s="2"/>
+      <c r="B139" s="3"/>
     </row>
     <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B140" s="2"/>
+      <c r="B140" s="3"/>
     </row>
     <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B141" s="2"/>
+      <c r="B141" s="3"/>
     </row>
     <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B142" s="2"/>
+      <c r="B142" s="3"/>
     </row>
     <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B143" s="2"/>
+      <c r="B143" s="3"/>
     </row>
     <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B144" s="2"/>
+      <c r="B144" s="3"/>
     </row>
     <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B145" s="2"/>
+      <c r="B145" s="3"/>
     </row>
     <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B146" s="2"/>
+      <c r="B146" s="3"/>
     </row>
     <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B147" s="2"/>
+      <c r="B147" s="3"/>
     </row>
     <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B148" s="2"/>
+      <c r="B148" s="3"/>
     </row>
     <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B149" s="2"/>
+      <c r="B149" s="3"/>
     </row>
     <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B150" s="2"/>
+      <c r="B150" s="3"/>
     </row>
     <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B151" s="2"/>
+      <c r="B151" s="3"/>
     </row>
     <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B152" s="2"/>
+      <c r="B152" s="3"/>
     </row>
     <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B153" s="2"/>
+      <c r="B153" s="3"/>
     </row>
     <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B154" s="2"/>
+      <c r="B154" s="3"/>
     </row>
     <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B155" s="2"/>
+      <c r="B155" s="3"/>
     </row>
     <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B156" s="2"/>
+      <c r="B156" s="3"/>
     </row>
     <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B157" s="2"/>
+      <c r="B157" s="3"/>
     </row>
     <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B158" s="2"/>
+      <c r="B158" s="3"/>
     </row>
     <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B159" s="2"/>
+      <c r="B159" s="3"/>
     </row>
     <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B160" s="2"/>
+      <c r="B160" s="3"/>
     </row>
     <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B161" s="2"/>
+      <c r="B161" s="3"/>
     </row>
     <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B162" s="2"/>
+      <c r="B162" s="3"/>
     </row>
     <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B163" s="2"/>
+      <c r="B163" s="3"/>
     </row>
     <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B164" s="2"/>
+      <c r="B164" s="3"/>
     </row>
     <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B165" s="2"/>
+      <c r="B165" s="3"/>
     </row>
     <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B166" s="2"/>
+      <c r="B166" s="3"/>
     </row>
     <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B167" s="2"/>
+      <c r="B167" s="3"/>
     </row>
     <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B168" s="2"/>
+      <c r="B168" s="3"/>
     </row>
     <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B169" s="2"/>
+      <c r="B169" s="3"/>
     </row>
     <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B170" s="2"/>
+      <c r="B170" s="3"/>
     </row>
     <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B171" s="2"/>
+      <c r="B171" s="3"/>
     </row>
     <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B172" s="2"/>
+      <c r="B172" s="3"/>
     </row>
     <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B173" s="2"/>
+      <c r="B173" s="3"/>
     </row>
     <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B174" s="2"/>
+      <c r="B174" s="3"/>
     </row>
     <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B175" s="2"/>
+      <c r="B175" s="3"/>
     </row>
     <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B176" s="2"/>
+      <c r="B176" s="3"/>
     </row>
     <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B177" s="2"/>
+      <c r="B177" s="3"/>
     </row>
     <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B178" s="2"/>
+      <c r="B178" s="3"/>
     </row>
     <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B179" s="2"/>
+      <c r="B179" s="3"/>
     </row>
     <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B180" s="2"/>
+      <c r="B180" s="3"/>
     </row>
     <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B181" s="2"/>
+      <c r="B181" s="3"/>
     </row>
     <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B182" s="2"/>
+      <c r="B182" s="3"/>
     </row>
     <row r="183" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B183" s="2"/>
+      <c r="B183" s="3"/>
     </row>
     <row r="184" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B184" s="2"/>
+      <c r="B184" s="3"/>
     </row>
     <row r="185" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B185" s="2"/>
+      <c r="B185" s="3"/>
     </row>
     <row r="186" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B186" s="2"/>
+      <c r="B186" s="3"/>
     </row>
     <row r="187" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B187" s="2"/>
+      <c r="B187" s="3"/>
     </row>
     <row r="188" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B188" s="2"/>
+      <c r="B188" s="3"/>
     </row>
     <row r="189" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B189" s="2"/>
+      <c r="B189" s="3"/>
     </row>
     <row r="190" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B190" s="2"/>
+      <c r="B190" s="3"/>
     </row>
     <row r="191" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B191" s="2"/>
+      <c r="B191" s="3"/>
     </row>
     <row r="192" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B192" s="2"/>
+      <c r="B192" s="3"/>
     </row>
     <row r="193" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B193" s="2"/>
+      <c r="B193" s="3"/>
     </row>
     <row r="194" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B194" s="2"/>
+      <c r="B194" s="3"/>
     </row>
     <row r="195" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B195" s="2"/>
+      <c r="B195" s="3"/>
     </row>
     <row r="196" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B196" s="2"/>
+      <c r="B196" s="3"/>
     </row>
     <row r="197" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B197" s="2"/>
+      <c r="B197" s="3"/>
     </row>
     <row r="198" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B198" s="2"/>
+      <c r="B198" s="3"/>
     </row>
     <row r="199" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B199" s="2"/>
+      <c r="B199" s="3"/>
     </row>
     <row r="200" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B200" s="2"/>
+      <c r="B200" s="3"/>
     </row>
     <row r="201" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B201" s="2"/>
+      <c r="B201" s="3"/>
     </row>
     <row r="202" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B202" s="2"/>
+      <c r="B202" s="3"/>
     </row>
     <row r="203" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B203" s="2"/>
+      <c r="B203" s="3"/>
     </row>
     <row r="204" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B204" s="2"/>
+      <c r="B204" s="3"/>
     </row>
     <row r="205" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B205" s="2"/>
+      <c r="B205" s="3"/>
     </row>
     <row r="206" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B206" s="2"/>
+      <c r="B206" s="3"/>
     </row>
     <row r="207" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B207" s="2"/>
+      <c r="B207" s="3"/>
     </row>
     <row r="208" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B208" s="2"/>
+      <c r="B208" s="3"/>
     </row>
     <row r="209" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B209" s="2"/>
+      <c r="B209" s="3"/>
     </row>
     <row r="210" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B210" s="2"/>
+      <c r="B210" s="3"/>
     </row>
     <row r="211" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B211" s="2"/>
+      <c r="B211" s="3"/>
     </row>
     <row r="212" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B212" s="2"/>
+      <c r="B212" s="3"/>
     </row>
     <row r="213" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B213" s="2"/>
+      <c r="B213" s="3"/>
     </row>
     <row r="214" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B214" s="2"/>
+      <c r="B214" s="3"/>
     </row>
     <row r="215" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B215" s="2"/>
+      <c r="B215" s="3"/>
     </row>
     <row r="216" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B216" s="2"/>
+      <c r="B216" s="3"/>
     </row>
     <row r="217" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B217" s="2"/>
+      <c r="B217" s="3"/>
     </row>
     <row r="218" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B218" s="2"/>
+      <c r="B218" s="3"/>
     </row>
     <row r="219" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B219" s="2"/>
+      <c r="B219" s="3"/>
     </row>
     <row r="220" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B220" s="2"/>
+      <c r="B220" s="3"/>
     </row>
     <row r="221" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B221" s="2"/>
+      <c r="B221" s="3"/>
     </row>
     <row r="222" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B222" s="2"/>
+      <c r="B222" s="3"/>
     </row>
     <row r="223" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B223" s="2"/>
+      <c r="B223" s="3"/>
     </row>
     <row r="224" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B224" s="2"/>
+      <c r="B224" s="3"/>
     </row>
     <row r="225" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B225" s="2"/>
+      <c r="B225" s="3"/>
     </row>
     <row r="226" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B226" s="2"/>
+      <c r="B226" s="3"/>
     </row>
     <row r="227" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B227" s="2"/>
+      <c r="B227" s="3"/>
     </row>
     <row r="228" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B228" s="2"/>
+      <c r="B228" s="3"/>
     </row>
     <row r="229" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B229" s="2"/>
+      <c r="B229" s="3"/>
     </row>
     <row r="230" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B230" s="2"/>
+      <c r="B230" s="3"/>
     </row>
     <row r="231" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B231" s="2"/>
+      <c r="B231" s="3"/>
     </row>
     <row r="232" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B232" s="2"/>
+      <c r="B232" s="3"/>
     </row>
     <row r="233" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B233" s="2"/>
+      <c r="B233" s="3"/>
     </row>
     <row r="234" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B234" s="2"/>
+      <c r="B234" s="3"/>
     </row>
     <row r="235" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B235" s="2"/>
+      <c r="B235" s="3"/>
     </row>
     <row r="236" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B236" s="2"/>
+      <c r="B236" s="3"/>
     </row>
     <row r="237" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B237" s="2"/>
+      <c r="B237" s="3"/>
     </row>
     <row r="238" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B238" s="2"/>
+      <c r="B238" s="3"/>
     </row>
     <row r="239" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B239" s="2"/>
+      <c r="B239" s="3"/>
     </row>
     <row r="240" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B240" s="2"/>
+      <c r="B240" s="3"/>
     </row>
     <row r="241" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B241" s="2"/>
+      <c r="B241" s="3"/>
     </row>
     <row r="242" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B242" s="2"/>
+      <c r="B242" s="3"/>
     </row>
     <row r="243" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B243" s="2"/>
+      <c r="B243" s="3"/>
     </row>
     <row r="244" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B244" s="2"/>
+      <c r="B244" s="3"/>
     </row>
     <row r="245" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B245" s="2"/>
+      <c r="B245" s="3"/>
     </row>
     <row r="246" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B246" s="2"/>
+      <c r="B246" s="3"/>
     </row>
     <row r="247" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B247" s="2"/>
+      <c r="B247" s="3"/>
     </row>
     <row r="248" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B248" s="2"/>
+      <c r="B248" s="3"/>
     </row>
     <row r="249" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B249" s="2"/>
+      <c r="B249" s="3"/>
     </row>
     <row r="250" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B250" s="2"/>
+      <c r="B250" s="3"/>
     </row>
     <row r="251" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B251" s="2"/>
+      <c r="B251" s="3"/>
     </row>
     <row r="252" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B252" s="2"/>
+      <c r="B252" s="3"/>
     </row>
     <row r="253" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B253" s="2"/>
+      <c r="B253" s="3"/>
     </row>
     <row r="254" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B254" s="2"/>
+      <c r="B254" s="3"/>
     </row>
     <row r="255" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B255" s="2"/>
+      <c r="B255" s="3"/>
     </row>
     <row r="256" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B256" s="2"/>
+      <c r="B256" s="3"/>
     </row>
     <row r="257" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B257" s="2"/>
+      <c r="B257" s="3"/>
     </row>
     <row r="258" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B258" s="2"/>
+      <c r="B258" s="3"/>
     </row>
     <row r="259" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B259" s="2"/>
+      <c r="B259" s="3"/>
     </row>
     <row r="260" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B260" s="2"/>
+      <c r="B260" s="3"/>
     </row>
     <row r="261" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B261" s="2"/>
+      <c r="B261" s="3"/>
     </row>
     <row r="262" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B262" s="2"/>
+      <c r="B262" s="3"/>
     </row>
     <row r="263" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B263" s="2"/>
+      <c r="B263" s="3"/>
     </row>
     <row r="264" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B264" s="2"/>
+      <c r="B264" s="3"/>
     </row>
     <row r="265" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B265" s="2"/>
+      <c r="B265" s="3"/>
     </row>
     <row r="266" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B266" s="2"/>
+      <c r="B266" s="3"/>
     </row>
     <row r="267" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B267" s="2"/>
+      <c r="B267" s="3"/>
     </row>
     <row r="268" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B268" s="2"/>
+      <c r="B268" s="3"/>
     </row>
     <row r="269" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B269" s="2"/>
+      <c r="B269" s="3"/>
     </row>
     <row r="270" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B270" s="2"/>
+      <c r="B270" s="3"/>
     </row>
     <row r="271" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B271" s="2"/>
+      <c r="B271" s="3"/>
     </row>
     <row r="272" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B272" s="2"/>
+      <c r="B272" s="3"/>
     </row>
     <row r="273" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B273" s="2"/>
+      <c r="B273" s="3"/>
     </row>
     <row r="274" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B274" s="2"/>
+      <c r="B274" s="3"/>
     </row>
     <row r="275" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B275" s="2"/>
+      <c r="B275" s="3"/>
     </row>
     <row r="276" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B276" s="2"/>
+      <c r="B276" s="3"/>
     </row>
     <row r="277" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B277" s="2"/>
+      <c r="B277" s="3"/>
     </row>
     <row r="278" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B278" s="2"/>
+      <c r="B278" s="3"/>
     </row>
     <row r="279" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B279" s="2"/>
+      <c r="B279" s="3"/>
     </row>
     <row r="280" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B280" s="2"/>
+      <c r="B280" s="3"/>
     </row>
     <row r="281" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B281" s="2"/>
+      <c r="B281" s="3"/>
     </row>
     <row r="282" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B282" s="2"/>
+      <c r="B282" s="3"/>
     </row>
     <row r="283" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B283" s="2"/>
+      <c r="B283" s="3"/>
     </row>
     <row r="284" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B284" s="2"/>
+      <c r="B284" s="3"/>
     </row>
     <row r="285" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B285" s="2"/>
+      <c r="B285" s="3"/>
     </row>
     <row r="286" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B286" s="2"/>
+      <c r="B286" s="3"/>
     </row>
     <row r="287" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B287" s="2"/>
+      <c r="B287" s="3"/>
     </row>
     <row r="288" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B288" s="2"/>
+      <c r="B288" s="3"/>
     </row>
     <row r="289" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B289" s="2"/>
+      <c r="B289" s="3"/>
     </row>
     <row r="290" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B290" s="2"/>
+      <c r="B290" s="3"/>
     </row>
     <row r="291" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B291" s="2"/>
+      <c r="B291" s="3"/>
     </row>
     <row r="292" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B292" s="2"/>
+      <c r="B292" s="3"/>
     </row>
     <row r="293" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B293" s="2"/>
+      <c r="B293" s="3"/>
     </row>
     <row r="294" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B294" s="2"/>
+      <c r="B294" s="3"/>
     </row>
     <row r="295" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B295" s="2"/>
+      <c r="B295" s="3"/>
     </row>
     <row r="296" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B296" s="2"/>
+      <c r="B296" s="3"/>
     </row>
     <row r="297" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B297" s="2"/>
+      <c r="B297" s="3"/>
     </row>
     <row r="298" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B298" s="2"/>
+      <c r="B298" s="3"/>
     </row>
     <row r="299" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B299" s="2"/>
+      <c r="B299" s="3"/>
     </row>
     <row r="300" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B300" s="2"/>
+      <c r="B300" s="3"/>
     </row>
     <row r="301" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B301" s="2"/>
+      <c r="B301" s="3"/>
     </row>
     <row r="302" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B302" s="2"/>
+      <c r="B302" s="3"/>
     </row>
     <row r="303" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B303" s="2"/>
+      <c r="B303" s="3"/>
     </row>
     <row r="304" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B304" s="2"/>
+      <c r="B304" s="3"/>
     </row>
     <row r="305" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B305" s="2"/>
+      <c r="B305" s="3"/>
     </row>
     <row r="306" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B306" s="2"/>
+      <c r="B306" s="3"/>
     </row>
     <row r="307" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B307" s="2"/>
+      <c r="B307" s="3"/>
     </row>
     <row r="308" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B308" s="2"/>
+      <c r="B308" s="3"/>
     </row>
     <row r="309" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B309" s="2"/>
+      <c r="B309" s="3"/>
     </row>
     <row r="310" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B310" s="2"/>
+      <c r="B310" s="3"/>
     </row>
     <row r="311" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B311" s="2"/>
+      <c r="B311" s="3"/>
     </row>
     <row r="312" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B312" s="2"/>
+      <c r="B312" s="3"/>
     </row>
     <row r="313" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B313" s="2"/>
+      <c r="B313" s="3"/>
     </row>
     <row r="314" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B314" s="2"/>
+      <c r="B314" s="3"/>
     </row>
     <row r="315" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B315" s="2"/>
+      <c r="B315" s="3"/>
     </row>
     <row r="316" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B316" s="2"/>
+      <c r="B316" s="3"/>
     </row>
     <row r="317" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B317" s="2"/>
+      <c r="B317" s="3"/>
     </row>
     <row r="318" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B318" s="2"/>
+      <c r="B318" s="3"/>
     </row>
     <row r="319" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B319" s="2"/>
+      <c r="B319" s="3"/>
     </row>
     <row r="320" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B320" s="2"/>
+      <c r="B320" s="3"/>
     </row>
     <row r="321" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B321" s="2"/>
+      <c r="B321" s="3"/>
     </row>
     <row r="322" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B322" s="2"/>
+      <c r="B322" s="3"/>
     </row>
     <row r="323" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B323" s="2"/>
+      <c r="B323" s="3"/>
     </row>
     <row r="324" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B324" s="2"/>
+      <c r="B324" s="3"/>
     </row>
     <row r="325" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B325" s="2"/>
+      <c r="B325" s="3"/>
     </row>
     <row r="326" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B326" s="2"/>
+      <c r="B326" s="3"/>
     </row>
     <row r="327" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B327" s="2"/>
+      <c r="B327" s="3"/>
     </row>
     <row r="328" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B328" s="2"/>
+      <c r="B328" s="3"/>
     </row>
     <row r="329" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B329" s="2"/>
+      <c r="B329" s="3"/>
     </row>
     <row r="330" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B330" s="2"/>
+      <c r="B330" s="3"/>
     </row>
     <row r="331" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B331" s="2"/>
+      <c r="B331" s="3"/>
     </row>
     <row r="332" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B332" s="2"/>
+      <c r="B332" s="3"/>
     </row>
     <row r="333" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B333" s="2"/>
+      <c r="B333" s="3"/>
     </row>
     <row r="334" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B334" s="2"/>
+      <c r="B334" s="3"/>
     </row>
     <row r="335" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B335" s="2"/>
+      <c r="B335" s="3"/>
     </row>
     <row r="336" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B336" s="2"/>
+      <c r="B336" s="3"/>
     </row>
     <row r="337" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B337" s="2"/>
+      <c r="B337" s="3"/>
     </row>
     <row r="338" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B338" s="2"/>
+      <c r="B338" s="3"/>
     </row>
     <row r="339" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B339" s="2"/>
+      <c r="B339" s="3"/>
     </row>
     <row r="340" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B340" s="2"/>
+      <c r="B340" s="3"/>
     </row>
     <row r="341" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B341" s="2"/>
+      <c r="B341" s="3"/>
     </row>
     <row r="342" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B342" s="2"/>
+      <c r="B342" s="3"/>
     </row>
     <row r="343" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B343" s="2"/>
+      <c r="B343" s="3"/>
     </row>
     <row r="344" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B344" s="2"/>
+      <c r="B344" s="3"/>
     </row>
     <row r="345" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B345" s="2"/>
+      <c r="B345" s="3"/>
     </row>
     <row r="346" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B346" s="2"/>
+      <c r="B346" s="3"/>
     </row>
     <row r="347" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B347" s="2"/>
+      <c r="B347" s="3"/>
     </row>
     <row r="348" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B348" s="2"/>
+      <c r="B348" s="3"/>
     </row>
     <row r="349" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B349" s="2"/>
+      <c r="B349" s="3"/>
     </row>
     <row r="350" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B350" s="2"/>
+      <c r="B350" s="3"/>
     </row>
     <row r="351" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B351" s="2"/>
+      <c r="B351" s="3"/>
     </row>
     <row r="352" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B352" s="2"/>
+      <c r="B352" s="3"/>
     </row>
     <row r="353" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B353" s="2"/>
+      <c r="B353" s="3"/>
     </row>
     <row r="354" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B354" s="2"/>
+      <c r="B354" s="3"/>
     </row>
     <row r="355" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B355" s="2"/>
+      <c r="B355" s="3"/>
     </row>
     <row r="356" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B356" s="2"/>
+      <c r="B356" s="3"/>
     </row>
     <row r="357" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B357" s="2"/>
+      <c r="B357" s="3"/>
     </row>
     <row r="358" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B358" s="2"/>
+      <c r="B358" s="3"/>
     </row>
     <row r="359" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B359" s="2"/>
+      <c r="B359" s="3"/>
     </row>
     <row r="360" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B360" s="2"/>
+      <c r="B360" s="3"/>
     </row>
     <row r="361" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B361" s="2"/>
+      <c r="B361" s="3"/>
     </row>
     <row r="362" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B362" s="2"/>
+      <c r="B362" s="3"/>
     </row>
     <row r="363" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B363" s="2"/>
+      <c r="B363" s="3"/>
     </row>
     <row r="364" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B364" s="2"/>
+      <c r="B364" s="3"/>
     </row>
     <row r="365" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B365" s="2"/>
+      <c r="B365" s="3"/>
     </row>
     <row r="366" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B366" s="2"/>
+      <c r="B366" s="3"/>
     </row>
     <row r="367" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B367" s="2"/>
+      <c r="B367" s="3"/>
     </row>
     <row r="368" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B368" s="2"/>
+      <c r="B368" s="3"/>
     </row>
     <row r="369" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B369" s="2"/>
+      <c r="B369" s="3"/>
     </row>
     <row r="370" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B370" s="2"/>
+      <c r="B370" s="3"/>
     </row>
     <row r="371" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B371" s="2"/>
+      <c r="B371" s="3"/>
     </row>
     <row r="372" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B372" s="2"/>
+      <c r="B372" s="3"/>
     </row>
     <row r="373" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B373" s="2"/>
+      <c r="B373" s="3"/>
     </row>
     <row r="374" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B374" s="2"/>
+      <c r="B374" s="3"/>
     </row>
     <row r="375" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B375" s="2"/>
+      <c r="B375" s="3"/>
     </row>
     <row r="376" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B376" s="2"/>
+      <c r="B376" s="3"/>
     </row>
     <row r="377" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B377" s="2"/>
+      <c r="B377" s="3"/>
     </row>
     <row r="378" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B378" s="2"/>
+      <c r="B378" s="3"/>
     </row>
     <row r="379" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B379" s="2"/>
+      <c r="B379" s="3"/>
     </row>
     <row r="380" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B380" s="2"/>
+      <c r="B380" s="3"/>
     </row>
     <row r="381" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B381" s="2"/>
+      <c r="B381" s="3"/>
     </row>
     <row r="382" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B382" s="2"/>
+      <c r="B382" s="3"/>
     </row>
     <row r="383" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B383" s="2"/>
+      <c r="B383" s="3"/>
     </row>
     <row r="384" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B384" s="2"/>
+      <c r="B384" s="3"/>
     </row>
     <row r="385" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B385" s="2"/>
+      <c r="B385" s="3"/>
     </row>
     <row r="386" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B386" s="2"/>
+      <c r="B386" s="3"/>
     </row>
     <row r="387" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B387" s="2"/>
+      <c r="B387" s="3"/>
     </row>
     <row r="388" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B388" s="2"/>
+      <c r="B388" s="3"/>
     </row>
     <row r="389" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B389" s="2"/>
+      <c r="B389" s="3"/>
     </row>
     <row r="390" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B390" s="2"/>
+      <c r="B390" s="3"/>
     </row>
     <row r="391" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B391" s="2"/>
+      <c r="B391" s="3"/>
     </row>
     <row r="392" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B392" s="2"/>
+      <c r="B392" s="3"/>
     </row>
     <row r="393" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B393" s="2"/>
+      <c r="B393" s="3"/>
     </row>
     <row r="394" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B394" s="2"/>
+      <c r="B394" s="3"/>
     </row>
     <row r="395" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B395" s="2"/>
+      <c r="B395" s="3"/>
     </row>
     <row r="396" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B396" s="2"/>
+      <c r="B396" s="3"/>
     </row>
     <row r="397" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B397" s="2"/>
+      <c r="B397" s="3"/>
     </row>
     <row r="398" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B398" s="2"/>
+      <c r="B398" s="3"/>
     </row>
     <row r="399" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B399" s="2"/>
+      <c r="B399" s="3"/>
     </row>
     <row r="400" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B400" s="2"/>
+      <c r="B400" s="3"/>
     </row>
     <row r="401" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B401" s="2"/>
+      <c r="B401" s="3"/>
     </row>
     <row r="402" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B402" s="2"/>
+      <c r="B402" s="3"/>
     </row>
     <row r="403" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B403" s="2"/>
+      <c r="B403" s="3"/>
     </row>
     <row r="404" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B404" s="2"/>
+      <c r="B404" s="3"/>
     </row>
     <row r="405" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B405" s="2"/>
+      <c r="B405" s="3"/>
     </row>
     <row r="406" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B406" s="2"/>
+      <c r="B406" s="3"/>
     </row>
     <row r="407" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B407" s="2"/>
+      <c r="B407" s="3"/>
     </row>
     <row r="408" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B408" s="2"/>
+      <c r="B408" s="3"/>
     </row>
     <row r="409" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B409" s="2"/>
+      <c r="B409" s="3"/>
     </row>
     <row r="410" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B410" s="2"/>
+      <c r="B410" s="3"/>
     </row>
     <row r="411" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B411" s="2"/>
+      <c r="B411" s="3"/>
     </row>
     <row r="412" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B412" s="2"/>
+      <c r="B412" s="3"/>
     </row>
     <row r="413" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B413" s="2"/>
+      <c r="B413" s="3"/>
     </row>
     <row r="414" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B414" s="2"/>
+      <c r="B414" s="3"/>
     </row>
     <row r="415" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B415" s="2"/>
+      <c r="B415" s="3"/>
     </row>
     <row r="416" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B416" s="2"/>
+      <c r="B416" s="3"/>
     </row>
     <row r="417" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B417" s="2"/>
+      <c r="B417" s="3"/>
     </row>
     <row r="418" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B418" s="2"/>
+      <c r="B418" s="3"/>
     </row>
     <row r="419" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B419" s="2"/>
+      <c r="B419" s="3"/>
     </row>
     <row r="420" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B420" s="2"/>
+      <c r="B420" s="3"/>
     </row>
     <row r="421" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B421" s="2"/>
+      <c r="B421" s="3"/>
     </row>
     <row r="422" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B422" s="2"/>
+      <c r="B422" s="3"/>
     </row>
     <row r="423" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B423" s="2"/>
+      <c r="B423" s="3"/>
     </row>
     <row r="424" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B424" s="2"/>
+      <c r="B424" s="3"/>
     </row>
     <row r="425" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B425" s="2"/>
+      <c r="B425" s="3"/>
     </row>
     <row r="426" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B426" s="2"/>
+      <c r="B426" s="3"/>
     </row>
     <row r="427" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B427" s="2"/>
+      <c r="B427" s="3"/>
     </row>
     <row r="428" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B428" s="2"/>
+      <c r="B428" s="3"/>
     </row>
     <row r="429" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B429" s="2"/>
+      <c r="B429" s="3"/>
     </row>
     <row r="430" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B430" s="2"/>
+      <c r="B430" s="3"/>
     </row>
     <row r="431" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B431" s="2"/>
+      <c r="B431" s="3"/>
     </row>
     <row r="432" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B432" s="2"/>
+      <c r="B432" s="3"/>
     </row>
     <row r="433" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B433" s="2"/>
+      <c r="B433" s="3"/>
     </row>
     <row r="434" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B434" s="2"/>
+      <c r="B434" s="3"/>
     </row>
     <row r="435" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B435" s="2"/>
+      <c r="B435" s="3"/>
     </row>
     <row r="436" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B436" s="2"/>
+      <c r="B436" s="3"/>
     </row>
     <row r="437" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B437" s="2"/>
+      <c r="B437" s="3"/>
     </row>
     <row r="438" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B438" s="2"/>
+      <c r="B438" s="3"/>
     </row>
     <row r="439" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B439" s="2"/>
+      <c r="B439" s="3"/>
     </row>
     <row r="440" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B440" s="2"/>
+      <c r="B440" s="3"/>
     </row>
     <row r="441" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B441" s="2"/>
+      <c r="B441" s="3"/>
     </row>
     <row r="442" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B442" s="2"/>
+      <c r="B442" s="3"/>
     </row>
     <row r="443" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B443" s="2"/>
+      <c r="B443" s="3"/>
     </row>
     <row r="444" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B444" s="2"/>
+      <c r="B444" s="3"/>
     </row>
     <row r="445" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B445" s="2"/>
+      <c r="B445" s="3"/>
     </row>
     <row r="446" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B446" s="2"/>
+      <c r="B446" s="3"/>
     </row>
     <row r="447" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B447" s="2"/>
+      <c r="B447" s="3"/>
     </row>
     <row r="448" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B448" s="2"/>
+      <c r="B448" s="3"/>
     </row>
     <row r="449" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B449" s="2"/>
+      <c r="B449" s="3"/>
     </row>
     <row r="450" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B450" s="2"/>
+      <c r="B450" s="3"/>
     </row>
     <row r="451" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B451" s="2"/>
+      <c r="B451" s="3"/>
     </row>
     <row r="452" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B452" s="2"/>
+      <c r="B452" s="3"/>
     </row>
     <row r="453" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B453" s="2"/>
+      <c r="B453" s="3"/>
     </row>
     <row r="454" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B454" s="2"/>
+      <c r="B454" s="3"/>
     </row>
     <row r="455" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B455" s="2"/>
+      <c r="B455" s="3"/>
     </row>
     <row r="456" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B456" s="2"/>
+      <c r="B456" s="3"/>
     </row>
     <row r="457" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B457" s="2"/>
+      <c r="B457" s="3"/>
     </row>
     <row r="458" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B458" s="2"/>
+      <c r="B458" s="3"/>
     </row>
     <row r="459" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B459" s="2"/>
+      <c r="B459" s="3"/>
     </row>
     <row r="460" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B460" s="2"/>
+      <c r="B460" s="3"/>
     </row>
     <row r="461" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B461" s="2"/>
+      <c r="B461" s="3"/>
     </row>
     <row r="462" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B462" s="2"/>
+      <c r="B462" s="3"/>
     </row>
     <row r="463" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B463" s="2"/>
+      <c r="B463" s="3"/>
     </row>
     <row r="464" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B464" s="2"/>
+      <c r="B464" s="3"/>
     </row>
     <row r="465" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B465" s="2"/>
+      <c r="B465" s="3"/>
     </row>
     <row r="466" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B466" s="2"/>
+      <c r="B466" s="3"/>
     </row>
     <row r="467" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B467" s="2"/>
+      <c r="B467" s="3"/>
     </row>
     <row r="468" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B468" s="2"/>
+      <c r="B468" s="3"/>
     </row>
     <row r="469" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B469" s="2"/>
+      <c r="B469" s="3"/>
     </row>
     <row r="470" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B470" s="2"/>
+      <c r="B470" s="3"/>
     </row>
     <row r="471" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B471" s="2"/>
+      <c r="B471" s="3"/>
     </row>
     <row r="472" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B472" s="2"/>
+      <c r="B472" s="3"/>
     </row>
     <row r="473" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B473" s="2"/>
+      <c r="B473" s="3"/>
     </row>
     <row r="474" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B474" s="2"/>
+      <c r="B474" s="3"/>
     </row>
     <row r="475" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B475" s="2"/>
+      <c r="B475" s="3"/>
     </row>
     <row r="476" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B476" s="2"/>
+      <c r="B476" s="3"/>
     </row>
     <row r="477" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B477" s="2"/>
+      <c r="B477" s="3"/>
     </row>
     <row r="478" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B478" s="2"/>
+      <c r="B478" s="3"/>
     </row>
     <row r="479" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B479" s="2"/>
+      <c r="B479" s="3"/>
     </row>
     <row r="480" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B480" s="2"/>
+      <c r="B480" s="3"/>
     </row>
     <row r="481" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B481" s="2"/>
+      <c r="B481" s="3"/>
     </row>
     <row r="482" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B482" s="2"/>
+      <c r="B482" s="3"/>
     </row>
     <row r="483" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B483" s="2"/>
+      <c r="B483" s="3"/>
     </row>
     <row r="484" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B484" s="2"/>
+      <c r="B484" s="3"/>
     </row>
     <row r="485" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B485" s="2"/>
+      <c r="B485" s="3"/>
     </row>
     <row r="486" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B486" s="2"/>
+      <c r="B486" s="3"/>
     </row>
     <row r="487" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B487" s="2"/>
+      <c r="B487" s="3"/>
     </row>
     <row r="488" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B488" s="2"/>
+      <c r="B488" s="3"/>
     </row>
     <row r="489" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B489" s="2"/>
+      <c r="B489" s="3"/>
     </row>
     <row r="490" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B490" s="2"/>
+      <c r="B490" s="3"/>
     </row>
     <row r="491" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B491" s="2"/>
+      <c r="B491" s="3"/>
     </row>
     <row r="492" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B492" s="2"/>
+      <c r="B492" s="3"/>
     </row>
     <row r="493" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B493" s="2"/>
+      <c r="B493" s="3"/>
     </row>
     <row r="494" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B494" s="2"/>
+      <c r="B494" s="3"/>
     </row>
     <row r="495" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B495" s="2"/>
+      <c r="B495" s="3"/>
     </row>
     <row r="496" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B496" s="2"/>
+      <c r="B496" s="3"/>
     </row>
     <row r="497" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B497" s="2"/>
+      <c r="B497" s="3"/>
     </row>
     <row r="498" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B498" s="2"/>
+      <c r="B498" s="3"/>
     </row>
     <row r="499" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B499" s="2"/>
+      <c r="B499" s="3"/>
     </row>
     <row r="500" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B500" s="2"/>
+      <c r="B500" s="3"/>
     </row>
     <row r="501" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B501" s="2"/>
+      <c r="B501" s="3"/>
     </row>
     <row r="502" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B502" s="2"/>
+      <c r="B502" s="3"/>
     </row>
     <row r="503" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B503" s="2"/>
+      <c r="B503" s="3"/>
     </row>
     <row r="504" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B504" s="2"/>
+      <c r="B504" s="3"/>
     </row>
     <row r="505" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B505" s="2"/>
+      <c r="B505" s="3"/>
     </row>
     <row r="506" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B506" s="2"/>
+      <c r="B506" s="3"/>
     </row>
     <row r="507" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B507" s="2"/>
+      <c r="B507" s="3"/>
     </row>
     <row r="508" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B508" s="2"/>
+      <c r="B508" s="3"/>
     </row>
     <row r="509" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B509" s="2"/>
+      <c r="B509" s="3"/>
     </row>
     <row r="510" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B510" s="2"/>
+      <c r="B510" s="3"/>
     </row>
     <row r="511" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B511" s="2"/>
+      <c r="B511" s="3"/>
     </row>
     <row r="512" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B512" s="2"/>
+      <c r="B512" s="3"/>
     </row>
     <row r="513" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B513" s="2"/>
+      <c r="B513" s="3"/>
     </row>
     <row r="514" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B514" s="2"/>
+      <c r="B514" s="3"/>
     </row>
     <row r="515" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B515" s="2"/>
+      <c r="B515" s="3"/>
     </row>
     <row r="516" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B516" s="2"/>
+      <c r="B516" s="3"/>
     </row>
     <row r="517" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B517" s="2"/>
+      <c r="B517" s="3"/>
     </row>
     <row r="518" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B518" s="2"/>
+      <c r="B518" s="3"/>
     </row>
     <row r="519" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B519" s="2"/>
+      <c r="B519" s="3"/>
     </row>
     <row r="520" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B520" s="2"/>
+      <c r="B520" s="3"/>
     </row>
     <row r="521" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B521" s="2"/>
+      <c r="B521" s="3"/>
     </row>
     <row r="522" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B522" s="2"/>
+      <c r="B522" s="3"/>
     </row>
     <row r="523" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B523" s="2"/>
+      <c r="B523" s="3"/>
     </row>
     <row r="524" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B524" s="2"/>
+      <c r="B524" s="3"/>
     </row>
     <row r="525" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B525" s="2"/>
+      <c r="B525" s="3"/>
     </row>
     <row r="526" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B526" s="2"/>
+      <c r="B526" s="3"/>
     </row>
     <row r="527" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B527" s="2"/>
+      <c r="B527" s="3"/>
     </row>
     <row r="528" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B528" s="2"/>
+      <c r="B528" s="3"/>
     </row>
     <row r="529" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B529" s="2"/>
+      <c r="B529" s="3"/>
     </row>
     <row r="530" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B530" s="2"/>
+      <c r="B530" s="3"/>
     </row>
     <row r="531" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B531" s="2"/>
+      <c r="B531" s="3"/>
     </row>
     <row r="532" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B532" s="2"/>
+      <c r="B532" s="3"/>
     </row>
     <row r="533" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B533" s="2"/>
+      <c r="B533" s="3"/>
     </row>
     <row r="534" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B534" s="2"/>
+      <c r="B534" s="3"/>
     </row>
     <row r="535" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B535" s="2"/>
+      <c r="B535" s="3"/>
     </row>
     <row r="536" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B536" s="2"/>
+      <c r="B536" s="3"/>
     </row>
     <row r="537" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B537" s="2"/>
+      <c r="B537" s="3"/>
     </row>
     <row r="538" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B538" s="2"/>
+      <c r="B538" s="3"/>
     </row>
     <row r="539" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B539" s="2"/>
+      <c r="B539" s="3"/>
     </row>
     <row r="540" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B540" s="2"/>
+      <c r="B540" s="3"/>
     </row>
     <row r="541" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B541" s="2"/>
+      <c r="B541" s="3"/>
     </row>
     <row r="542" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B542" s="2"/>
+      <c r="B542" s="3"/>
     </row>
     <row r="543" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B543" s="2"/>
+      <c r="B543" s="3"/>
     </row>
     <row r="544" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B544" s="2"/>
+      <c r="B544" s="3"/>
     </row>
     <row r="545" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B545" s="2"/>
+      <c r="B545" s="3"/>
     </row>
     <row r="546" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B546" s="2"/>
+      <c r="B546" s="3"/>
     </row>
     <row r="547" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B547" s="2"/>
+      <c r="B547" s="3"/>
     </row>
     <row r="548" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B548" s="2"/>
+      <c r="B548" s="3"/>
     </row>
     <row r="549" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B549" s="2"/>
+      <c r="B549" s="3"/>
     </row>
     <row r="550" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B550" s="2"/>
+      <c r="B550" s="3"/>
     </row>
     <row r="551" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B551" s="2"/>
+      <c r="B551" s="3"/>
     </row>
     <row r="552" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B552" s="2"/>
+      <c r="B552" s="3"/>
     </row>
     <row r="553" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B553" s="2"/>
+      <c r="B553" s="3"/>
     </row>
     <row r="554" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B554" s="2"/>
+      <c r="B554" s="3"/>
     </row>
     <row r="555" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B555" s="2"/>
+      <c r="B555" s="3"/>
     </row>
     <row r="556" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B556" s="2"/>
+      <c r="B556" s="3"/>
     </row>
     <row r="557" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B557" s="2"/>
+      <c r="B557" s="3"/>
     </row>
     <row r="558" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B558" s="2"/>
+      <c r="B558" s="3"/>
     </row>
     <row r="559" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B559" s="2"/>
+      <c r="B559" s="3"/>
     </row>
     <row r="560" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B560" s="2"/>
+      <c r="B560" s="3"/>
     </row>
     <row r="561" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B561" s="2"/>
+      <c r="B561" s="3"/>
     </row>
     <row r="562" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B562" s="2"/>
+      <c r="B562" s="3"/>
     </row>
     <row r="563" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B563" s="2"/>
+      <c r="B563" s="3"/>
     </row>
     <row r="564" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B564" s="2"/>
+      <c r="B564" s="3"/>
     </row>
     <row r="565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B565" s="2"/>
+      <c r="B565" s="3"/>
     </row>
     <row r="566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B566" s="2"/>
+      <c r="B566" s="3"/>
     </row>
     <row r="567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B567" s="2"/>
+      <c r="B567" s="3"/>
     </row>
     <row r="568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B568" s="2"/>
+      <c r="B568" s="3"/>
     </row>
     <row r="569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B569" s="2"/>
+      <c r="B569" s="3"/>
     </row>
     <row r="570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B570" s="2"/>
+      <c r="B570" s="3"/>
     </row>
     <row r="571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B571" s="2"/>
+      <c r="B571" s="3"/>
     </row>
     <row r="572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B572" s="2"/>
+      <c r="B572" s="3"/>
     </row>
     <row r="573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B573" s="2"/>
+      <c r="B573" s="3"/>
     </row>
     <row r="574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B574" s="2"/>
+      <c r="B574" s="3"/>
     </row>
     <row r="575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B575" s="2"/>
+      <c r="B575" s="3"/>
     </row>
     <row r="576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B576" s="2"/>
+      <c r="B576" s="3"/>
     </row>
     <row r="577" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B577" s="2"/>
+      <c r="B577" s="3"/>
     </row>
     <row r="578" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B578" s="2"/>
+      <c r="B578" s="3"/>
     </row>
     <row r="579" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B579" s="2"/>
+      <c r="B579" s="3"/>
     </row>
     <row r="580" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B580" s="2"/>
+      <c r="B580" s="3"/>
     </row>
     <row r="581" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B581" s="2"/>
+      <c r="B581" s="3"/>
     </row>
     <row r="582" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B582" s="2"/>
+      <c r="B582" s="3"/>
     </row>
     <row r="583" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B583" s="2"/>
+      <c r="B583" s="3"/>
     </row>
     <row r="584" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B584" s="2"/>
+      <c r="B584" s="3"/>
     </row>
     <row r="585" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B585" s="2"/>
+      <c r="B585" s="3"/>
     </row>
     <row r="586" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B586" s="2"/>
+      <c r="B586" s="3"/>
     </row>
     <row r="587" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B587" s="2"/>
+      <c r="B587" s="3"/>
     </row>
     <row r="588" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B588" s="2"/>
+      <c r="B588" s="3"/>
     </row>
     <row r="589" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B589" s="2"/>
+      <c r="B589" s="3"/>
     </row>
     <row r="590" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B590" s="2"/>
+      <c r="B590" s="3"/>
     </row>
     <row r="591" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B591" s="2"/>
+      <c r="B591" s="3"/>
     </row>
     <row r="592" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B592" s="2"/>
+      <c r="B592" s="3"/>
     </row>
     <row r="593" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B593" s="2"/>
+      <c r="B593" s="3"/>
     </row>
     <row r="594" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B594" s="2"/>
+      <c r="B594" s="3"/>
     </row>
     <row r="595" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B595" s="2"/>
+      <c r="B595" s="3"/>
     </row>
     <row r="596" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B596" s="2"/>
+      <c r="B596" s="3"/>
     </row>
     <row r="597" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B597" s="2"/>
+      <c r="B597" s="3"/>
     </row>
     <row r="598" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B598" s="2"/>
+      <c r="B598" s="3"/>
     </row>
     <row r="599" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B599" s="2"/>
+      <c r="B599" s="3"/>
     </row>
     <row r="600" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B600" s="2"/>
+      <c r="B600" s="3"/>
     </row>
     <row r="601" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B601" s="2"/>
+      <c r="B601" s="3"/>
     </row>
     <row r="602" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B602" s="2"/>
+      <c r="B602" s="3"/>
     </row>
     <row r="603" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B603" s="2"/>
+      <c r="B603" s="3"/>
     </row>
     <row r="604" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B604" s="2"/>
+      <c r="B604" s="3"/>
     </row>
     <row r="605" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B605" s="2"/>
+      <c r="B605" s="3"/>
     </row>
     <row r="606" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B606" s="2"/>
+      <c r="B606" s="3"/>
     </row>
     <row r="607" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B607" s="2"/>
+      <c r="B607" s="3"/>
     </row>
     <row r="608" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B608" s="2"/>
+      <c r="B608" s="3"/>
     </row>
     <row r="609" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B609" s="2"/>
+      <c r="B609" s="3"/>
     </row>
     <row r="610" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B610" s="2"/>
+      <c r="B610" s="3"/>
     </row>
     <row r="611" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B611" s="2"/>
+      <c r="B611" s="3"/>
     </row>
     <row r="612" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B612" s="2"/>
+      <c r="B612" s="3"/>
     </row>
     <row r="613" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B613" s="2"/>
+      <c r="B613" s="3"/>
     </row>
     <row r="614" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B614" s="2"/>
+      <c r="B614" s="3"/>
     </row>
     <row r="615" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B615" s="2"/>
+      <c r="B615" s="3"/>
     </row>
     <row r="616" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B616" s="2"/>
+      <c r="B616" s="3"/>
     </row>
     <row r="617" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B617" s="2"/>
+      <c r="B617" s="3"/>
     </row>
     <row r="618" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B618" s="2"/>
+      <c r="B618" s="3"/>
     </row>
     <row r="619" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B619" s="2"/>
+      <c r="B619" s="3"/>
     </row>
     <row r="620" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B620" s="2"/>
+      <c r="B620" s="3"/>
     </row>
     <row r="621" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B621" s="2"/>
+      <c r="B621" s="3"/>
     </row>
     <row r="622" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B622" s="2"/>
+      <c r="B622" s="3"/>
     </row>
     <row r="623" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B623" s="2"/>
+      <c r="B623" s="3"/>
     </row>
     <row r="624" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B624" s="2"/>
+      <c r="B624" s="3"/>
     </row>
     <row r="625" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B625" s="2"/>
+      <c r="B625" s="3"/>
     </row>
     <row r="626" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B626" s="2"/>
+      <c r="B626" s="3"/>
     </row>
     <row r="627" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B627" s="2"/>
+      <c r="B627" s="3"/>
     </row>
     <row r="628" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B628" s="2"/>
+      <c r="B628" s="3"/>
     </row>
     <row r="629" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B629" s="2"/>
+      <c r="B629" s="3"/>
     </row>
     <row r="630" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B630" s="2"/>
+      <c r="B630" s="3"/>
     </row>
     <row r="631" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B631" s="2"/>
+      <c r="B631" s="3"/>
     </row>
     <row r="632" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B632" s="2"/>
+      <c r="B632" s="3"/>
     </row>
     <row r="633" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B633" s="2"/>
+      <c r="B633" s="3"/>
     </row>
     <row r="634" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B634" s="2"/>
+      <c r="B634" s="3"/>
     </row>
     <row r="635" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B635" s="2"/>
+      <c r="B635" s="3"/>
     </row>
     <row r="636" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B636" s="2"/>
+      <c r="B636" s="3"/>
     </row>
     <row r="637" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B637" s="2"/>
+      <c r="B637" s="3"/>
     </row>
     <row r="638" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B638" s="2"/>
+      <c r="B638" s="3"/>
     </row>
     <row r="639" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B639" s="2"/>
+      <c r="B639" s="3"/>
     </row>
     <row r="640" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B640" s="2"/>
+      <c r="B640" s="3"/>
     </row>
     <row r="641" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B641" s="2"/>
+      <c r="B641" s="3"/>
     </row>
     <row r="642" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B642" s="2"/>
+      <c r="B642" s="3"/>
     </row>
     <row r="643" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B643" s="2"/>
+      <c r="B643" s="3"/>
     </row>
     <row r="644" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B644" s="2"/>
+      <c r="B644" s="3"/>
     </row>
     <row r="645" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B645" s="2"/>
+      <c r="B645" s="3"/>
     </row>
     <row r="646" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B646" s="2"/>
+      <c r="B646" s="3"/>
     </row>
     <row r="647" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B647" s="2"/>
+      <c r="B647" s="3"/>
     </row>
     <row r="648" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B648" s="2"/>
+      <c r="B648" s="3"/>
     </row>
     <row r="649" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B649" s="2"/>
+      <c r="B649" s="3"/>
     </row>
     <row r="650" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B650" s="2"/>
+      <c r="B650" s="3"/>
     </row>
     <row r="651" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B651" s="2"/>
+      <c r="B651" s="3"/>
     </row>
     <row r="652" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B652" s="2"/>
+      <c r="B652" s="3"/>
     </row>
     <row r="653" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B653" s="2"/>
+      <c r="B653" s="3"/>
     </row>
     <row r="654" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B654" s="2"/>
+      <c r="B654" s="3"/>
     </row>
     <row r="655" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B655" s="2"/>
+      <c r="B655" s="3"/>
     </row>
     <row r="656" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B656" s="2"/>
+      <c r="B656" s="3"/>
     </row>
     <row r="657" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B657" s="2"/>
+      <c r="B657" s="3"/>
     </row>
     <row r="658" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B658" s="2"/>
+      <c r="B658" s="3"/>
     </row>
     <row r="659" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B659" s="2"/>
+      <c r="B659" s="3"/>
     </row>
     <row r="660" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B660" s="2"/>
+      <c r="B660" s="3"/>
     </row>
     <row r="661" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B661" s="2"/>
+      <c r="B661" s="3"/>
     </row>
     <row r="662" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B662" s="2"/>
+      <c r="B662" s="3"/>
     </row>
     <row r="663" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B663" s="2"/>
+      <c r="B663" s="3"/>
     </row>
     <row r="664" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B664" s="2"/>
+      <c r="B664" s="3"/>
     </row>
     <row r="665" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B665" s="2"/>
+      <c r="B665" s="3"/>
     </row>
     <row r="666" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B666" s="2"/>
+      <c r="B666" s="3"/>
     </row>
     <row r="667" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B667" s="2"/>
+      <c r="B667" s="3"/>
     </row>
     <row r="668" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B668" s="2"/>
+      <c r="B668" s="3"/>
     </row>
     <row r="669" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B669" s="2"/>
+      <c r="B669" s="3"/>
     </row>
     <row r="670" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B670" s="2"/>
+      <c r="B670" s="3"/>
     </row>
     <row r="671" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B671" s="2"/>
+      <c r="B671" s="3"/>
     </row>
     <row r="672" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B672" s="2"/>
+      <c r="B672" s="3"/>
     </row>
     <row r="673" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B673" s="2"/>
+      <c r="B673" s="3"/>
     </row>
     <row r="674" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B674" s="2"/>
+      <c r="B674" s="3"/>
     </row>
     <row r="675" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B675" s="2"/>
+      <c r="B675" s="3"/>
     </row>
     <row r="676" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B676" s="2"/>
+      <c r="B676" s="3"/>
     </row>
     <row r="677" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B677" s="2"/>
+      <c r="B677" s="3"/>
     </row>
     <row r="678" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B678" s="2"/>
+      <c r="B678" s="3"/>
     </row>
     <row r="679" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B679" s="2"/>
+      <c r="B679" s="3"/>
     </row>
     <row r="680" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B680" s="2"/>
+      <c r="B680" s="3"/>
     </row>
     <row r="681" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B681" s="2"/>
+      <c r="B681" s="3"/>
     </row>
     <row r="682" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B682" s="2"/>
+      <c r="B682" s="3"/>
     </row>
     <row r="683" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B683" s="2"/>
+      <c r="B683" s="3"/>
     </row>
     <row r="684" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B684" s="2"/>
+      <c r="B684" s="3"/>
     </row>
     <row r="685" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B685" s="2"/>
+      <c r="B685" s="3"/>
     </row>
     <row r="686" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B686" s="2"/>
+      <c r="B686" s="3"/>
     </row>
     <row r="687" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B687" s="2"/>
+      <c r="B687" s="3"/>
     </row>
     <row r="688" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B688" s="2"/>
+      <c r="B688" s="3"/>
     </row>
     <row r="689" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B689" s="2"/>
+      <c r="B689" s="3"/>
     </row>
     <row r="690" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B690" s="2"/>
+      <c r="B690" s="3"/>
     </row>
     <row r="691" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B691" s="2"/>
+      <c r="B691" s="3"/>
     </row>
     <row r="692" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B692" s="2"/>
+      <c r="B692" s="3"/>
     </row>
     <row r="693" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B693" s="2"/>
+      <c r="B693" s="3"/>
     </row>
     <row r="694" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B694" s="2"/>
+      <c r="B694" s="3"/>
     </row>
     <row r="695" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B695" s="2"/>
+      <c r="B695" s="3"/>
     </row>
     <row r="696" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B696" s="2"/>
+      <c r="B696" s="3"/>
     </row>
     <row r="697" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B697" s="2"/>
+      <c r="B697" s="3"/>
     </row>
     <row r="698" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B698" s="2"/>
+      <c r="B698" s="3"/>
     </row>
     <row r="699" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B699" s="2"/>
+      <c r="B699" s="3"/>
     </row>
     <row r="700" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B700" s="2"/>
+      <c r="B700" s="3"/>
     </row>
     <row r="701" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B701" s="2"/>
+      <c r="B701" s="3"/>
     </row>
     <row r="702" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B702" s="2"/>
+      <c r="B702" s="3"/>
     </row>
     <row r="703" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B703" s="2"/>
+      <c r="B703" s="3"/>
     </row>
     <row r="704" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B704" s="2"/>
+      <c r="B704" s="3"/>
     </row>
     <row r="705" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B705" s="2"/>
+      <c r="B705" s="3"/>
     </row>
     <row r="706" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B706" s="2"/>
+      <c r="B706" s="3"/>
     </row>
     <row r="707" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B707" s="2"/>
+      <c r="B707" s="3"/>
     </row>
     <row r="708" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B708" s="2"/>
+      <c r="B708" s="3"/>
     </row>
     <row r="709" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B709" s="2"/>
+      <c r="B709" s="3"/>
     </row>
     <row r="710" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B710" s="2"/>
+      <c r="B710" s="3"/>
     </row>
     <row r="711" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B711" s="2"/>
+      <c r="B711" s="3"/>
     </row>
     <row r="712" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B712" s="2"/>
+      <c r="B712" s="3"/>
     </row>
     <row r="713" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B713" s="2"/>
+      <c r="B713" s="3"/>
     </row>
     <row r="714" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B714" s="2"/>
+      <c r="B714" s="3"/>
     </row>
     <row r="715" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B715" s="2"/>
+      <c r="B715" s="3"/>
     </row>
     <row r="716" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B716" s="2"/>
+      <c r="B716" s="3"/>
     </row>
     <row r="717" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B717" s="2"/>
+      <c r="B717" s="3"/>
     </row>
     <row r="718" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B718" s="2"/>
+      <c r="B718" s="3"/>
     </row>
     <row r="719" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B719" s="2"/>
+      <c r="B719" s="3"/>
     </row>
     <row r="720" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B720" s="2"/>
+      <c r="B720" s="3"/>
     </row>
     <row r="721" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B721" s="2"/>
+      <c r="B721" s="3"/>
     </row>
     <row r="722" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B722" s="2"/>
+      <c r="B722" s="3"/>
     </row>
     <row r="723" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B723" s="2"/>
+      <c r="B723" s="3"/>
     </row>
     <row r="724" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B724" s="2"/>
+      <c r="B724" s="3"/>
     </row>
     <row r="725" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B725" s="2"/>
+      <c r="B725" s="3"/>
     </row>
     <row r="726" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B726" s="2"/>
+      <c r="B726" s="3"/>
     </row>
     <row r="727" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B727" s="2"/>
+      <c r="B727" s="3"/>
     </row>
     <row r="728" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B728" s="2"/>
+      <c r="B728" s="3"/>
     </row>
     <row r="729" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B729" s="2"/>
+      <c r="B729" s="3"/>
     </row>
     <row r="730" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B730" s="2"/>
+      <c r="B730" s="3"/>
     </row>
     <row r="731" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B731" s="2"/>
+      <c r="B731" s="3"/>
     </row>
     <row r="732" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B732" s="2"/>
+      <c r="B732" s="3"/>
     </row>
     <row r="733" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B733" s="2"/>
+      <c r="B733" s="3"/>
     </row>
     <row r="734" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B734" s="2"/>
+      <c r="B734" s="3"/>
     </row>
     <row r="735" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B735" s="2"/>
+      <c r="B735" s="3"/>
     </row>
     <row r="736" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B736" s="2"/>
+      <c r="B736" s="3"/>
     </row>
     <row r="737" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B737" s="2"/>
+      <c r="B737" s="3"/>
     </row>
     <row r="738" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B738" s="2"/>
+      <c r="B738" s="3"/>
     </row>
     <row r="739" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B739" s="2"/>
+      <c r="B739" s="3"/>
     </row>
     <row r="740" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B740" s="2"/>
+      <c r="B740" s="3"/>
     </row>
     <row r="741" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B741" s="2"/>
+      <c r="B741" s="3"/>
     </row>
     <row r="742" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B742" s="2"/>
+      <c r="B742" s="3"/>
     </row>
     <row r="743" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B743" s="2"/>
+      <c r="B743" s="3"/>
     </row>
     <row r="744" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B744" s="2"/>
+      <c r="B744" s="3"/>
     </row>
     <row r="745" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B745" s="2"/>
+      <c r="B745" s="3"/>
     </row>
     <row r="746" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B746" s="2"/>
+      <c r="B746" s="3"/>
     </row>
     <row r="747" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B747" s="2"/>
+      <c r="B747" s="3"/>
     </row>
     <row r="748" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B748" s="2"/>
+      <c r="B748" s="3"/>
     </row>
     <row r="749" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B749" s="2"/>
+      <c r="B749" s="3"/>
     </row>
     <row r="750" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B750" s="2"/>
+      <c r="B750" s="3"/>
     </row>
     <row r="751" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B751" s="2"/>
+      <c r="B751" s="3"/>
     </row>
     <row r="752" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B752" s="2"/>
+      <c r="B752" s="3"/>
     </row>
     <row r="753" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B753" s="2"/>
+      <c r="B753" s="3"/>
     </row>
     <row r="754" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B754" s="2"/>
+      <c r="B754" s="3"/>
     </row>
     <row r="755" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B755" s="2"/>
+      <c r="B755" s="3"/>
     </row>
     <row r="756" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B756" s="2"/>
+      <c r="B756" s="3"/>
     </row>
     <row r="757" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B757" s="2"/>
+      <c r="B757" s="3"/>
     </row>
     <row r="758" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B758" s="2"/>
+      <c r="B758" s="3"/>
     </row>
     <row r="759" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B759" s="2"/>
+      <c r="B759" s="3"/>
     </row>
     <row r="760" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B760" s="2"/>
+      <c r="B760" s="3"/>
     </row>
     <row r="761" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B761" s="2"/>
+      <c r="B761" s="3"/>
     </row>
     <row r="762" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B762" s="2"/>
+      <c r="B762" s="3"/>
     </row>
     <row r="763" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B763" s="2"/>
+      <c r="B763" s="3"/>
     </row>
     <row r="764" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B764" s="2"/>
+      <c r="B764" s="3"/>
     </row>
     <row r="765" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B765" s="2"/>
+      <c r="B765" s="3"/>
     </row>
     <row r="766" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B766" s="2"/>
+      <c r="B766" s="3"/>
     </row>
     <row r="767" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B767" s="2"/>
+      <c r="B767" s="3"/>
     </row>
     <row r="768" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B768" s="2"/>
+      <c r="B768" s="3"/>
     </row>
     <row r="769" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B769" s="2"/>
+      <c r="B769" s="3"/>
     </row>
     <row r="770" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B770" s="2"/>
+      <c r="B770" s="3"/>
     </row>
     <row r="771" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B771" s="2"/>
+      <c r="B771" s="3"/>
     </row>
     <row r="772" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B772" s="2"/>
+      <c r="B772" s="3"/>
     </row>
     <row r="773" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B773" s="2"/>
+      <c r="B773" s="3"/>
     </row>
     <row r="774" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B774" s="2"/>
+      <c r="B774" s="3"/>
     </row>
     <row r="775" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B775" s="2"/>
+      <c r="B775" s="3"/>
     </row>
     <row r="776" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B776" s="2"/>
+      <c r="B776" s="3"/>
     </row>
     <row r="777" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B777" s="2"/>
+      <c r="B777" s="3"/>
     </row>
     <row r="778" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B778" s="2"/>
+      <c r="B778" s="3"/>
     </row>
     <row r="779" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B779" s="2"/>
+      <c r="B779" s="3"/>
     </row>
     <row r="780" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B780" s="2"/>
+      <c r="B780" s="3"/>
     </row>
     <row r="781" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B781" s="2"/>
+      <c r="B781" s="3"/>
     </row>
     <row r="782" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B782" s="2"/>
+      <c r="B782" s="3"/>
     </row>
     <row r="783" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B783" s="2"/>
+      <c r="B783" s="3"/>
     </row>
     <row r="784" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B784" s="2"/>
+      <c r="B784" s="3"/>
     </row>
     <row r="785" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B785" s="2"/>
+      <c r="B785" s="3"/>
     </row>
     <row r="786" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B786" s="2"/>
+      <c r="B786" s="3"/>
     </row>
     <row r="787" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B787" s="2"/>
+      <c r="B787" s="3"/>
     </row>
     <row r="788" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B788" s="2"/>
+      <c r="B788" s="3"/>
     </row>
     <row r="789" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B789" s="2"/>
+      <c r="B789" s="3"/>
     </row>
     <row r="790" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B790" s="2"/>
+      <c r="B790" s="3"/>
     </row>
     <row r="791" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B791" s="2"/>
+      <c r="B791" s="3"/>
     </row>
     <row r="792" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B792" s="2"/>
+      <c r="B792" s="3"/>
     </row>
     <row r="793" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B793" s="2"/>
+      <c r="B793" s="3"/>
     </row>
     <row r="794" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B794" s="2"/>
+      <c r="B794" s="3"/>
     </row>
     <row r="795" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B795" s="2"/>
+      <c r="B795" s="3"/>
     </row>
     <row r="796" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B796" s="2"/>
+      <c r="B796" s="3"/>
     </row>
     <row r="797" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B797" s="2"/>
+      <c r="B797" s="3"/>
     </row>
     <row r="798" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B798" s="2"/>
+      <c r="B798" s="3"/>
     </row>
     <row r="799" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B799" s="2"/>
+      <c r="B799" s="3"/>
     </row>
     <row r="800" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B800" s="2"/>
+      <c r="B800" s="3"/>
     </row>
     <row r="801" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B801" s="2"/>
+      <c r="B801" s="3"/>
     </row>
     <row r="802" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B802" s="2"/>
+      <c r="B802" s="3"/>
     </row>
     <row r="803" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B803" s="2"/>
+      <c r="B803" s="3"/>
     </row>
     <row r="804" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B804" s="2"/>
+      <c r="B804" s="3"/>
     </row>
     <row r="805" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B805" s="2"/>
+      <c r="B805" s="3"/>
     </row>
     <row r="806" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B806" s="2"/>
+      <c r="B806" s="3"/>
     </row>
     <row r="807" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B807" s="2"/>
+      <c r="B807" s="3"/>
     </row>
     <row r="808" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B808" s="2"/>
+      <c r="B808" s="3"/>
     </row>
     <row r="809" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B809" s="2"/>
+      <c r="B809" s="3"/>
     </row>
     <row r="810" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B810" s="2"/>
+      <c r="B810" s="3"/>
     </row>
     <row r="811" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B811" s="2"/>
+      <c r="B811" s="3"/>
     </row>
     <row r="812" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B812" s="2"/>
+      <c r="B812" s="3"/>
     </row>
     <row r="813" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B813" s="2"/>
+      <c r="B813" s="3"/>
     </row>
     <row r="814" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B814" s="2"/>
+      <c r="B814" s="3"/>
     </row>
     <row r="815" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B815" s="2"/>
+      <c r="B815" s="3"/>
     </row>
     <row r="816" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B816" s="2"/>
+      <c r="B816" s="3"/>
     </row>
     <row r="817" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B817" s="2"/>
+      <c r="B817" s="3"/>
     </row>
     <row r="818" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B818" s="2"/>
+      <c r="B818" s="3"/>
     </row>
     <row r="819" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B819" s="2"/>
+      <c r="B819" s="3"/>
     </row>
     <row r="820" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B820" s="2"/>
+      <c r="B820" s="3"/>
     </row>
     <row r="821" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B821" s="2"/>
+      <c r="B821" s="3"/>
     </row>
     <row r="822" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B822" s="2"/>
+      <c r="B822" s="3"/>
     </row>
     <row r="823" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B823" s="2"/>
+      <c r="B823" s="3"/>
     </row>
     <row r="824" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B824" s="2"/>
+      <c r="B824" s="3"/>
     </row>
     <row r="825" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B825" s="2"/>
+      <c r="B825" s="3"/>
     </row>
     <row r="826" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B826" s="2"/>
+      <c r="B826" s="3"/>
     </row>
     <row r="827" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B827" s="2"/>
+      <c r="B827" s="3"/>
     </row>
     <row r="828" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B828" s="2"/>
+      <c r="B828" s="3"/>
     </row>
     <row r="829" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B829" s="2"/>
+      <c r="B829" s="3"/>
     </row>
     <row r="830" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B830" s="2"/>
+      <c r="B830" s="3"/>
     </row>
     <row r="831" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B831" s="2"/>
+      <c r="B831" s="3"/>
     </row>
     <row r="832" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B832" s="2"/>
+      <c r="B832" s="3"/>
     </row>
     <row r="833" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B833" s="2"/>
+      <c r="B833" s="3"/>
     </row>
     <row r="834" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B834" s="2"/>
+      <c r="B834" s="3"/>
     </row>
     <row r="835" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B835" s="2"/>
+      <c r="B835" s="3"/>
     </row>
     <row r="836" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B836" s="2"/>
+      <c r="B836" s="3"/>
     </row>
     <row r="837" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B837" s="2"/>
+      <c r="B837" s="3"/>
     </row>
     <row r="838" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B838" s="2"/>
+      <c r="B838" s="3"/>
     </row>
     <row r="839" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B839" s="2"/>
+      <c r="B839" s="3"/>
     </row>
     <row r="840" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B840" s="2"/>
+      <c r="B840" s="3"/>
     </row>
     <row r="841" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B841" s="2"/>
+      <c r="B841" s="3"/>
     </row>
     <row r="842" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B842" s="2"/>
+      <c r="B842" s="3"/>
     </row>
     <row r="843" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B843" s="2"/>
+      <c r="B843" s="3"/>
     </row>
     <row r="844" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B844" s="2"/>
+      <c r="B844" s="3"/>
     </row>
     <row r="845" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B845" s="2"/>
+      <c r="B845" s="3"/>
     </row>
     <row r="846" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B846" s="2"/>
+      <c r="B846" s="3"/>
     </row>
     <row r="847" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B847" s="2"/>
+      <c r="B847" s="3"/>
     </row>
     <row r="848" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B848" s="2"/>
+      <c r="B848" s="3"/>
     </row>
     <row r="849" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B849" s="2"/>
+      <c r="B849" s="3"/>
     </row>
     <row r="850" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B850" s="2"/>
+      <c r="B850" s="3"/>
     </row>
     <row r="851" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B851" s="2"/>
+      <c r="B851" s="3"/>
     </row>
     <row r="852" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B852" s="2"/>
+      <c r="B852" s="3"/>
     </row>
     <row r="853" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B853" s="2"/>
+      <c r="B853" s="3"/>
     </row>
     <row r="854" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B854" s="2"/>
+      <c r="B854" s="3"/>
     </row>
     <row r="855" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B855" s="2"/>
+      <c r="B855" s="3"/>
     </row>
     <row r="856" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B856" s="2"/>
+      <c r="B856" s="3"/>
     </row>
     <row r="857" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B857" s="2"/>
+      <c r="B857" s="3"/>
     </row>
     <row r="858" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B858" s="2"/>
+      <c r="B858" s="3"/>
     </row>
     <row r="859" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B859" s="2"/>
+      <c r="B859" s="3"/>
     </row>
     <row r="860" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B860" s="2"/>
+      <c r="B860" s="3"/>
     </row>
     <row r="861" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B861" s="2"/>
+      <c r="B861" s="3"/>
     </row>
     <row r="862" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B862" s="2"/>
+      <c r="B862" s="3"/>
     </row>
     <row r="863" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B863" s="2"/>
+      <c r="B863" s="3"/>
     </row>
     <row r="864" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B864" s="2"/>
+      <c r="B864" s="3"/>
     </row>
     <row r="865" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B865" s="2"/>
+      <c r="B865" s="3"/>
     </row>
     <row r="866" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B866" s="2"/>
+      <c r="B866" s="3"/>
     </row>
     <row r="867" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B867" s="2"/>
+      <c r="B867" s="3"/>
     </row>
     <row r="868" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B868" s="2"/>
+      <c r="B868" s="3"/>
     </row>
     <row r="869" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B869" s="2"/>
+      <c r="B869" s="3"/>
     </row>
     <row r="870" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B870" s="2"/>
+      <c r="B870" s="3"/>
     </row>
     <row r="871" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B871" s="2"/>
+      <c r="B871" s="3"/>
     </row>
     <row r="872" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B872" s="2"/>
+      <c r="B872" s="3"/>
     </row>
     <row r="873" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B873" s="2"/>
+      <c r="B873" s="3"/>
     </row>
     <row r="874" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B874" s="2"/>
+      <c r="B874" s="3"/>
     </row>
     <row r="875" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B875" s="2"/>
+      <c r="B875" s="3"/>
     </row>
     <row r="876" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B876" s="2"/>
+      <c r="B876" s="3"/>
     </row>
     <row r="877" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B877" s="2"/>
+      <c r="B877" s="3"/>
     </row>
     <row r="878" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B878" s="2"/>
+      <c r="B878" s="3"/>
     </row>
     <row r="879" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B879" s="2"/>
+      <c r="B879" s="3"/>
     </row>
     <row r="880" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B880" s="2"/>
+      <c r="B880" s="3"/>
     </row>
     <row r="881" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B881" s="2"/>
+      <c r="B881" s="3"/>
     </row>
     <row r="882" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B882" s="2"/>
+      <c r="B882" s="3"/>
     </row>
     <row r="883" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B883" s="2"/>
+      <c r="B883" s="3"/>
     </row>
     <row r="884" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B884" s="2"/>
+      <c r="B884" s="3"/>
     </row>
     <row r="885" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B885" s="2"/>
+      <c r="B885" s="3"/>
     </row>
     <row r="886" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B886" s="2"/>
+      <c r="B886" s="3"/>
     </row>
     <row r="887" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B887" s="2"/>
+      <c r="B887" s="3"/>
     </row>
     <row r="888" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B888" s="2"/>
+      <c r="B888" s="3"/>
     </row>
     <row r="889" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B889" s="2"/>
+      <c r="B889" s="3"/>
     </row>
     <row r="890" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B890" s="2"/>
+      <c r="B890" s="3"/>
     </row>
     <row r="891" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B891" s="2"/>
+      <c r="B891" s="3"/>
     </row>
     <row r="892" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B892" s="2"/>
+      <c r="B892" s="3"/>
     </row>
     <row r="893" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B893" s="2"/>
+      <c r="B893" s="3"/>
     </row>
     <row r="894" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B894" s="2"/>
+      <c r="B894" s="3"/>
     </row>
     <row r="895" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B895" s="2"/>
+      <c r="B895" s="3"/>
     </row>
     <row r="896" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B896" s="2"/>
+      <c r="B896" s="3"/>
     </row>
     <row r="897" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B897" s="2"/>
+      <c r="B897" s="3"/>
     </row>
     <row r="898" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B898" s="2"/>
+      <c r="B898" s="3"/>
     </row>
     <row r="899" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B899" s="2"/>
+      <c r="B899" s="3"/>
     </row>
     <row r="900" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B900" s="2"/>
+      <c r="B900" s="3"/>
     </row>
     <row r="901" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B901" s="2"/>
+      <c r="B901" s="3"/>
     </row>
     <row r="902" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B902" s="2"/>
+      <c r="B902" s="3"/>
     </row>
     <row r="903" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B903" s="2"/>
+      <c r="B903" s="3"/>
     </row>
     <row r="904" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B904" s="2"/>
+      <c r="B904" s="3"/>
     </row>
     <row r="905" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B905" s="2"/>
+      <c r="B905" s="3"/>
     </row>
     <row r="906" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B906" s="2"/>
+      <c r="B906" s="3"/>
     </row>
     <row r="907" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B907" s="2"/>
+      <c r="B907" s="3"/>
     </row>
     <row r="908" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B908" s="2"/>
+      <c r="B908" s="3"/>
     </row>
     <row r="909" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B909" s="2"/>
+      <c r="B909" s="3"/>
     </row>
     <row r="910" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B910" s="2"/>
+      <c r="B910" s="3"/>
     </row>
     <row r="911" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B911" s="2"/>
+      <c r="B911" s="3"/>
     </row>
     <row r="912" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B912" s="2"/>
+      <c r="B912" s="3"/>
     </row>
     <row r="913" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B913" s="2"/>
+      <c r="B913" s="3"/>
     </row>
     <row r="914" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B914" s="2"/>
+      <c r="B914" s="3"/>
     </row>
     <row r="915" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B915" s="2"/>
+      <c r="B915" s="3"/>
     </row>
     <row r="916" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B916" s="2"/>
+      <c r="B916" s="3"/>
     </row>
     <row r="917" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B917" s="2"/>
+      <c r="B917" s="3"/>
     </row>
     <row r="918" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B918" s="2"/>
+      <c r="B918" s="3"/>
     </row>
     <row r="919" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B919" s="2"/>
+      <c r="B919" s="3"/>
     </row>
     <row r="920" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B920" s="2"/>
+      <c r="B920" s="3"/>
     </row>
     <row r="921" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B921" s="2"/>
+      <c r="B921" s="3"/>
     </row>
     <row r="922" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B922" s="2"/>
+      <c r="B922" s="3"/>
     </row>
     <row r="923" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B923" s="2"/>
+      <c r="B923" s="3"/>
     </row>
     <row r="924" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B924" s="2"/>
+      <c r="B924" s="3"/>
     </row>
     <row r="925" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B925" s="2"/>
+      <c r="B925" s="3"/>
     </row>
     <row r="926" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B926" s="2"/>
+      <c r="B926" s="3"/>
     </row>
     <row r="927" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B927" s="2"/>
+      <c r="B927" s="3"/>
     </row>
     <row r="928" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B928" s="2"/>
+      <c r="B928" s="3"/>
     </row>
     <row r="929" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B929" s="2"/>
+      <c r="B929" s="3"/>
     </row>
     <row r="930" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B930" s="2"/>
+      <c r="B930" s="3"/>
     </row>
     <row r="931" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B931" s="2"/>
+      <c r="B931" s="3"/>
     </row>
     <row r="932" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B932" s="2"/>
+      <c r="B932" s="3"/>
     </row>
     <row r="933" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B933" s="2"/>
+      <c r="B933" s="3"/>
     </row>
     <row r="934" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B934" s="2"/>
+      <c r="B934" s="3"/>
     </row>
     <row r="935" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B935" s="2"/>
+      <c r="B935" s="3"/>
     </row>
     <row r="936" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B936" s="2"/>
+      <c r="B936" s="3"/>
     </row>
     <row r="937" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B937" s="2"/>
+      <c r="B937" s="3"/>
     </row>
     <row r="938" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B938" s="2"/>
+      <c r="B938" s="3"/>
     </row>
     <row r="939" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B939" s="2"/>
+      <c r="B939" s="3"/>
     </row>
     <row r="940" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B940" s="2"/>
+      <c r="B940" s="3"/>
     </row>
     <row r="941" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B941" s="2"/>
+      <c r="B941" s="3"/>
     </row>
     <row r="942" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B942" s="2"/>
+      <c r="B942" s="3"/>
     </row>
     <row r="943" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B943" s="2"/>
+      <c r="B943" s="3"/>
     </row>
     <row r="944" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B944" s="2"/>
+      <c r="B944" s="3"/>
     </row>
     <row r="945" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B945" s="2"/>
+      <c r="B945" s="3"/>
     </row>
     <row r="946" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B946" s="2"/>
+      <c r="B946" s="3"/>
     </row>
     <row r="947" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B947" s="2"/>
+      <c r="B947" s="3"/>
     </row>
     <row r="948" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B948" s="2"/>
+      <c r="B948" s="3"/>
     </row>
     <row r="949" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B949" s="2"/>
+      <c r="B949" s="3"/>
     </row>
     <row r="950" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B950" s="2"/>
+      <c r="B950" s="3"/>
     </row>
     <row r="951" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B951" s="2"/>
+      <c r="B951" s="3"/>
     </row>
     <row r="952" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B952" s="2"/>
+      <c r="B952" s="3"/>
     </row>
     <row r="953" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B953" s="2"/>
+      <c r="B953" s="3"/>
     </row>
     <row r="954" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B954" s="2"/>
+      <c r="B954" s="3"/>
     </row>
     <row r="955" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B955" s="2"/>
+      <c r="B955" s="3"/>
     </row>
     <row r="956" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B956" s="2"/>
+      <c r="B956" s="3"/>
     </row>
     <row r="957" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B957" s="2"/>
+      <c r="B957" s="3"/>
     </row>
     <row r="958" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B958" s="2"/>
+      <c r="B958" s="3"/>
     </row>
     <row r="959" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B959" s="2"/>
+      <c r="B959" s="3"/>
     </row>
     <row r="960" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B960" s="2"/>
+      <c r="B960" s="3"/>
     </row>
     <row r="961" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B961" s="2"/>
+      <c r="B961" s="3"/>
     </row>
     <row r="962" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B962" s="2"/>
+      <c r="B962" s="3"/>
     </row>
     <row r="963" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B963" s="2"/>
+      <c r="B963" s="3"/>
     </row>
     <row r="964" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B964" s="2"/>
+      <c r="B964" s="3"/>
     </row>
     <row r="965" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B965" s="2"/>
+      <c r="B965" s="3"/>
     </row>
     <row r="966" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B966" s="2"/>
+      <c r="B966" s="3"/>
     </row>
     <row r="967" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B967" s="2"/>
+      <c r="B967" s="3"/>
     </row>
     <row r="968" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B968" s="2"/>
+      <c r="B968" s="3"/>
     </row>
     <row r="969" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B969" s="2"/>
+      <c r="B969" s="3"/>
     </row>
     <row r="970" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B970" s="2"/>
+      <c r="B970" s="3"/>
     </row>
     <row r="971" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B971" s="2"/>
+      <c r="B971" s="3"/>
     </row>
     <row r="972" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B972" s="2"/>
+      <c r="B972" s="3"/>
     </row>
     <row r="973" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B973" s="2"/>
+      <c r="B973" s="3"/>
     </row>
     <row r="974" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B974" s="2"/>
+      <c r="B974" s="3"/>
     </row>
     <row r="975" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B975" s="2"/>
+      <c r="B975" s="3"/>
     </row>
     <row r="976" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B976" s="2"/>
+      <c r="B976" s="3"/>
     </row>
     <row r="977" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B977" s="2"/>
+      <c r="B977" s="3"/>
     </row>
     <row r="978" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B978" s="2"/>
+      <c r="B978" s="3"/>
     </row>
     <row r="979" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B979" s="2"/>
+      <c r="B979" s="3"/>
     </row>
     <row r="980" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B980" s="2"/>
+      <c r="B980" s="3"/>
     </row>
     <row r="981" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B981" s="2"/>
+      <c r="B981" s="3"/>
     </row>
     <row r="982" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B982" s="2"/>
+      <c r="B982" s="3"/>
     </row>
     <row r="983" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B983" s="2"/>
+      <c r="B983" s="3"/>
     </row>
     <row r="984" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B984" s="2"/>
+      <c r="B984" s="3"/>
     </row>
     <row r="985" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B985" s="2"/>
+      <c r="B985" s="3"/>
     </row>
     <row r="986" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B986" s="2"/>
+      <c r="B986" s="3"/>
     </row>
     <row r="987" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B987" s="2"/>
+      <c r="B987" s="3"/>
     </row>
     <row r="988" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B988" s="2"/>
+      <c r="B988" s="3"/>
     </row>
     <row r="989" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B989" s="2"/>
+      <c r="B989" s="3"/>
     </row>
     <row r="990" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B990" s="2"/>
+      <c r="B990" s="3"/>
     </row>
     <row r="991" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B991" s="2"/>
+      <c r="B991" s="3"/>
     </row>
     <row r="992" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B992" s="2"/>
+      <c r="B992" s="3"/>
     </row>
     <row r="993" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B993" s="2"/>
+      <c r="B993" s="3"/>
     </row>
     <row r="994" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B994" s="2"/>
+      <c r="B994" s="3"/>
     </row>
     <row r="995" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B995" s="2"/>
+      <c r="B995" s="3"/>
     </row>
     <row r="996" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B996" s="2"/>
+      <c r="B996" s="3"/>
     </row>
     <row r="997" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B997" s="2"/>
+      <c r="B997" s="3"/>
     </row>
     <row r="998" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B998" s="2"/>
+      <c r="B998" s="3"/>
     </row>
     <row r="999" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B999" s="2"/>
+      <c r="B999" s="3"/>
     </row>
     <row r="1000" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1000" s="2"/>
+      <c r="B1000" s="3"/>
     </row>
     <row r="1001" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1001" s="2"/>
+      <c r="B1001" s="3"/>
     </row>
     <row r="1002" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1002" s="2"/>
+      <c r="B1002" s="3"/>
     </row>
     <row r="1003" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1003" s="2"/>
+      <c r="B1003" s="3"/>
     </row>
     <row r="1004" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1004" s="2"/>
+      <c r="B1004" s="3"/>
     </row>
     <row r="1005" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1005" s="2"/>
+      <c r="B1005" s="3"/>
     </row>
     <row r="1006" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1006" s="2"/>
+      <c r="B1006" s="3"/>
     </row>
     <row r="1007" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1007" s="2"/>
+      <c r="B1007" s="3"/>
     </row>
     <row r="1008" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1008" s="2"/>
+      <c r="B1008" s="3"/>
     </row>
     <row r="1009" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1009" s="2"/>
+      <c r="B1009" s="3"/>
     </row>
     <row r="1010" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1010" s="2"/>
+      <c r="B1010" s="3"/>
     </row>
     <row r="1011" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1011" s="2"/>
+      <c r="B1011" s="3"/>
     </row>
     <row r="1012" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1012" s="2"/>
+      <c r="B1012" s="3"/>
     </row>
     <row r="1013" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1013" s="2"/>
+      <c r="B1013" s="3"/>
     </row>
     <row r="1014" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1014" s="2"/>
+      <c r="B1014" s="3"/>
     </row>
     <row r="1015" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1015" s="2"/>
+      <c r="B1015" s="3"/>
     </row>
     <row r="1016" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1016" s="2"/>
-    </row>
-    <row r="1017" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1017" s="2"/>
+      <c r="B1016" s="3"/>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B3:B1017" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B3:B1016" type="list">
       <formula1>Data!$A$2:$A$4</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -3427,7 +3526,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -3437,21 +3536,21 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" customHeight="false" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>12</v>
+      <c r="A3" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>10</v>
+      <c r="A4" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>